<commit_message>
Soil Forecast Model Included
</commit_message>
<xml_diff>
--- a/data/Soil_temperature_forecast_10_days.xlsx
+++ b/data/Soil_temperature_forecast_10_days.xlsx
@@ -523,22 +523,22 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45405</v>
+        <v>45411</v>
       </c>
       <c r="B2" t="n">
-        <v>6.6</v>
+        <v>7.8125</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.7</v>
+        <v>3.5</v>
       </c>
       <c r="D2" t="n">
-        <v>9.699999999999999</v>
+        <v>10.5</v>
       </c>
       <c r="E2" t="n">
-        <v>53.2</v>
+        <v>88.175</v>
       </c>
       <c r="F2" t="n">
-        <v>1001.269807013271</v>
+        <v>1011.051944743122</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -550,45 +550,45 @@
         <v>4</v>
       </c>
       <c r="J2" t="n">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="K2" t="n">
-        <v>5.268000000000004</v>
+        <v>5.791377543624169</v>
       </c>
       <c r="L2" t="n">
-        <v>5.210006090084254</v>
+        <v>5.677516843120022</v>
       </c>
       <c r="M2" t="n">
-        <v>5.062366650016652</v>
+        <v>5.595194113481074</v>
       </c>
       <c r="N2" t="n">
-        <v>4.758946111039802</v>
+        <v>5.151161093946595</v>
       </c>
       <c r="O2" t="n">
-        <v>4.009689088689089</v>
+        <v>4.521395945090218</v>
       </c>
       <c r="P2" t="n">
-        <v>3.43025360757234</v>
+        <v>3.420377619647766</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45406</v>
+        <v>45412</v>
       </c>
       <c r="B3" t="n">
-        <v>4.745833333333333</v>
+        <v>9.725</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.7</v>
+        <v>3.5</v>
       </c>
       <c r="D3" t="n">
-        <v>8.6</v>
+        <v>14.3</v>
       </c>
       <c r="E3" t="n">
-        <v>65.3</v>
+        <v>89.21249999999999</v>
       </c>
       <c r="F3" t="n">
-        <v>998.2877700202605</v>
+        <v>1015.850915142929</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -600,145 +600,145 @@
         <v>4</v>
       </c>
       <c r="J3" t="n">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="K3" t="n">
-        <v>4.928000000000003</v>
+        <v>7.353811737318463</v>
       </c>
       <c r="L3" t="n">
-        <v>4.926683333333333</v>
+        <v>7.25727072305879</v>
       </c>
       <c r="M3" t="n">
-        <v>4.968419667559517</v>
+        <v>7.142052262331761</v>
       </c>
       <c r="N3" t="n">
-        <v>4.959837293262295</v>
+        <v>6.515144020162255</v>
       </c>
       <c r="O3" t="n">
-        <v>4.944745507270508</v>
+        <v>5.39911823591947</v>
       </c>
       <c r="P3" t="n">
-        <v>3.965862172471206</v>
+        <v>4.15617515858971</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45407</v>
+        <v>45413</v>
       </c>
       <c r="B4" t="n">
-        <v>4.057142857142857</v>
+        <v>11.4875</v>
       </c>
       <c r="C4" t="n">
-        <v>1.7</v>
+        <v>6.2</v>
       </c>
       <c r="D4" t="n">
-        <v>8.6</v>
+        <v>16.3</v>
       </c>
       <c r="E4" t="n">
-        <v>89.89285714285714</v>
+        <v>68.6875</v>
       </c>
       <c r="F4" t="n">
-        <v>995.764366772918</v>
+        <v>1014.289883072826</v>
       </c>
       <c r="G4" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J4" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="K4" t="n">
-        <v>4.806000000000003</v>
+        <v>9.746383534853404</v>
       </c>
       <c r="L4" t="n">
-        <v>4.751257395382393</v>
+        <v>9.583914022080549</v>
       </c>
       <c r="M4" t="n">
-        <v>4.606244805194804</v>
+        <v>9.455973997361156</v>
       </c>
       <c r="N4" t="n">
-        <v>4.862563195357275</v>
+        <v>9.000052572493837</v>
       </c>
       <c r="O4" t="n">
-        <v>4.107985522810522</v>
+        <v>7.964533447735224</v>
       </c>
       <c r="P4" t="n">
-        <v>3.500563835734271</v>
+        <v>6.161662057835041</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45408</v>
+        <v>45414</v>
       </c>
       <c r="B5" t="n">
-        <v>4.1</v>
+        <v>14.225</v>
       </c>
       <c r="C5" t="n">
-        <v>1.5</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="D5" t="n">
-        <v>5.9</v>
+        <v>19.8</v>
       </c>
       <c r="E5" t="n">
-        <v>92.15000000000001</v>
+        <v>67.59999999999999</v>
       </c>
       <c r="F5" t="n">
-        <v>990.8548785771535</v>
+        <v>1010.095566015488</v>
       </c>
       <c r="G5" t="n">
-        <v>1.15</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J5" t="n">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="K5" t="n">
-        <v>4.504777777777779</v>
+        <v>11.17226086676881</v>
       </c>
       <c r="L5" t="n">
-        <v>4.3209826038083</v>
+        <v>10.96551109576654</v>
       </c>
       <c r="M5" t="n">
-        <v>4.165563769563772</v>
+        <v>10.79630447786615</v>
       </c>
       <c r="N5" t="n">
-        <v>4.048021393790883</v>
+        <v>10.14202901156393</v>
       </c>
       <c r="O5" t="n">
-        <v>3.638590965947149</v>
+        <v>9.009832640559624</v>
       </c>
       <c r="P5" t="n">
-        <v>3.132292646242647</v>
+        <v>6.941975406800601</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45409</v>
+        <v>45415</v>
       </c>
       <c r="B6" t="n">
-        <v>6</v>
+        <v>14.4</v>
       </c>
       <c r="C6" t="n">
-        <v>1.1</v>
+        <v>7.2</v>
       </c>
       <c r="D6" t="n">
-        <v>9.199999999999999</v>
+        <v>19.7</v>
       </c>
       <c r="E6" t="n">
-        <v>80.825</v>
+        <v>69</v>
       </c>
       <c r="F6" t="n">
-        <v>996.814830045116</v>
+        <v>1006.789173293079</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
@@ -747,48 +747,48 @@
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J6" t="n">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="K6" t="n">
-        <v>5.595000000000003</v>
+        <v>11.20551190392998</v>
       </c>
       <c r="L6" t="n">
-        <v>5.43202028447129</v>
+        <v>11.02469714287919</v>
       </c>
       <c r="M6" t="n">
-        <v>5.462169946570314</v>
+        <v>10.85969954574997</v>
       </c>
       <c r="N6" t="n">
-        <v>4.981283874458874</v>
+        <v>10.17898013612291</v>
       </c>
       <c r="O6" t="n">
-        <v>4.944745507270508</v>
+        <v>9.092596766998762</v>
       </c>
       <c r="P6" t="n">
-        <v>3.965862172471206</v>
+        <v>6.889598149941348</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45410</v>
+        <v>45416</v>
       </c>
       <c r="B7" t="n">
-        <v>8.449999999999999</v>
+        <v>14.475</v>
       </c>
       <c r="C7" t="n">
-        <v>0.9</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="D7" t="n">
-        <v>13.2</v>
+        <v>19.5</v>
       </c>
       <c r="E7" t="n">
-        <v>77.575</v>
+        <v>64.47499999999999</v>
       </c>
       <c r="F7" t="n">
-        <v>1005.862009214</v>
+        <v>1005.061298545689</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
@@ -797,148 +797,148 @@
         <v>0</v>
       </c>
       <c r="I7" t="n">
+        <v>5</v>
+      </c>
+      <c r="J7" t="n">
         <v>4</v>
       </c>
-      <c r="J7" t="n">
-        <v>28</v>
-      </c>
       <c r="K7" t="n">
-        <v>5.253000000000001</v>
+        <v>11.13823833034559</v>
       </c>
       <c r="L7" t="n">
-        <v>5.210006090084254</v>
+        <v>10.94169111688645</v>
       </c>
       <c r="M7" t="n">
-        <v>5.062366650016652</v>
+        <v>10.76945745094702</v>
       </c>
       <c r="N7" t="n">
-        <v>4.758946111039802</v>
+        <v>10.13997430765606</v>
       </c>
       <c r="O7" t="n">
-        <v>4.009689088689089</v>
+        <v>9.009780719034444</v>
       </c>
       <c r="P7" t="n">
-        <v>3.43025360757234</v>
+        <v>6.94197507760016</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45411</v>
+        <v>45417</v>
       </c>
       <c r="B8" t="n">
-        <v>10.15</v>
+        <v>12.625</v>
       </c>
       <c r="C8" t="n">
-        <v>5.6</v>
+        <v>7</v>
       </c>
       <c r="D8" t="n">
-        <v>13</v>
+        <v>16.9</v>
       </c>
       <c r="E8" t="n">
-        <v>81.75</v>
+        <v>66.5</v>
       </c>
       <c r="F8" t="n">
-        <v>1010.058551324141</v>
+        <v>1008.178773733112</v>
       </c>
       <c r="G8" t="n">
-        <v>0.675</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J8" t="n">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="K8" t="n">
-        <v>5.579000000000002</v>
+        <v>10.71249358589029</v>
       </c>
       <c r="L8" t="n">
-        <v>5.43202028447129</v>
+        <v>10.56510486885183</v>
       </c>
       <c r="M8" t="n">
-        <v>5.462169946570314</v>
+        <v>10.57740809076677</v>
       </c>
       <c r="N8" t="n">
-        <v>4.981283874458874</v>
+        <v>10.05278383724556</v>
       </c>
       <c r="O8" t="n">
-        <v>4.944745507270508</v>
+        <v>9.007577451601327</v>
       </c>
       <c r="P8" t="n">
-        <v>3.965862172471206</v>
+        <v>6.941961108122077</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45412</v>
+        <v>45418</v>
       </c>
       <c r="B9" t="n">
-        <v>11.2</v>
+        <v>11.4</v>
       </c>
       <c r="C9" t="n">
-        <v>6.7</v>
+        <v>5.8</v>
       </c>
       <c r="D9" t="n">
-        <v>14.2</v>
+        <v>15.7</v>
       </c>
       <c r="E9" t="n">
-        <v>86.82499999999999</v>
+        <v>70.65000000000001</v>
       </c>
       <c r="F9" t="n">
-        <v>1011.509547612217</v>
+        <v>1009.267751964902</v>
       </c>
       <c r="G9" t="n">
-        <v>1.175</v>
+        <v>0</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J9" t="n">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="K9" t="n">
-        <v>6.836000000000005</v>
+        <v>9.878128359683625</v>
       </c>
       <c r="L9" t="n">
-        <v>6.621189940614943</v>
+        <v>9.802533281050177</v>
       </c>
       <c r="M9" t="n">
-        <v>6.328726984126982</v>
+        <v>9.723369469326094</v>
       </c>
       <c r="N9" t="n">
-        <v>5.759403948828949</v>
+        <v>9.087083711455918</v>
       </c>
       <c r="O9" t="n">
-        <v>5.097822979797979</v>
+        <v>8.157014119254471</v>
       </c>
       <c r="P9" t="n">
-        <v>4.182516608391608</v>
+        <v>5.909927118985828</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>45413</v>
+        <v>45419</v>
       </c>
       <c r="B10" t="n">
-        <v>11.825</v>
+        <v>11.225</v>
       </c>
       <c r="C10" t="n">
-        <v>6.9</v>
+        <v>5.6</v>
       </c>
       <c r="D10" t="n">
-        <v>15.3</v>
+        <v>15</v>
       </c>
       <c r="E10" t="n">
-        <v>83.40000000000001</v>
+        <v>66.75</v>
       </c>
       <c r="F10" t="n">
-        <v>1010.446531095385</v>
+        <v>1010.941929630209</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
@@ -950,45 +950,45 @@
         <v>5</v>
       </c>
       <c r="J10" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="K10" t="n">
-        <v>10.544</v>
+        <v>9.742964699829432</v>
       </c>
       <c r="L10" t="n">
-        <v>10.24523824345589</v>
+        <v>9.583144016141574</v>
       </c>
       <c r="M10" t="n">
-        <v>10.0377094443611</v>
+        <v>9.455724787595667</v>
       </c>
       <c r="N10" t="n">
-        <v>9.361406349206348</v>
+        <v>9.00003349953352</v>
       </c>
       <c r="O10" t="n">
-        <v>8.520698987532075</v>
+        <v>7.964532965769338</v>
       </c>
       <c r="P10" t="n">
-        <v>6.335430103230106</v>
+        <v>6.16166205477921</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>45414</v>
+        <v>45420</v>
       </c>
       <c r="B11" t="n">
-        <v>12.875</v>
+        <v>11.075</v>
       </c>
       <c r="C11" t="n">
-        <v>7</v>
+        <v>6.8</v>
       </c>
       <c r="D11" t="n">
-        <v>16.7</v>
+        <v>13.9</v>
       </c>
       <c r="E11" t="n">
-        <v>76.52500000000001</v>
+        <v>72</v>
       </c>
       <c r="F11" t="n">
-        <v>1006.779312094767</v>
+        <v>1011.306800285849</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
@@ -1000,45 +1000,45 @@
         <v>5</v>
       </c>
       <c r="J11" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="K11" t="n">
-        <v>11.16099999999999</v>
+        <v>10.03086049699492</v>
       </c>
       <c r="L11" t="n">
-        <v>10.90028418002276</v>
+        <v>9.901546065648002</v>
       </c>
       <c r="M11" t="n">
-        <v>10.61978246328834</v>
+        <v>9.823226181482399</v>
       </c>
       <c r="N11" t="n">
-        <v>9.938865767432599</v>
+        <v>9.454338332837597</v>
       </c>
       <c r="O11" t="n">
-        <v>9.259589351446628</v>
+        <v>8.305700911365102</v>
       </c>
       <c r="P11" t="n">
-        <v>7.153115007265581</v>
+        <v>6.353378191254905</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>45415</v>
+        <v>45421</v>
       </c>
       <c r="B12" t="n">
-        <v>9.65</v>
+        <v>11.83333333333333</v>
       </c>
       <c r="C12" t="n">
-        <v>7.1</v>
+        <v>7</v>
       </c>
       <c r="D12" t="n">
-        <v>10.5</v>
+        <v>16.4</v>
       </c>
       <c r="E12" t="n">
-        <v>84.8</v>
+        <v>73.96666666666667</v>
       </c>
       <c r="F12" t="n">
-        <v>1008.308074500602</v>
+        <v>1010.90011243065</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
@@ -1050,25 +1050,25 @@
         <v>5</v>
       </c>
       <c r="J12" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="K12" t="n">
-        <v>8.798999999999999</v>
+        <v>10.92125957150249</v>
       </c>
       <c r="L12" t="n">
-        <v>8.698700472974743</v>
+        <v>10.75432625041842</v>
       </c>
       <c r="M12" t="n">
-        <v>8.67085165945166</v>
+        <v>10.65353229403615</v>
       </c>
       <c r="N12" t="n">
-        <v>8.274149603174605</v>
+        <v>10.08450872932704</v>
       </c>
       <c r="O12" t="n">
-        <v>7.577588766788766</v>
+        <v>9.008379126614813</v>
       </c>
       <c r="P12" t="n">
-        <v>5.934614364024344</v>
+        <v>6.941966191019125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>